<commit_message>
added test files and examples
</commit_message>
<xml_diff>
--- a/Test c#/Parts.xlsx
+++ b/Test c#/Parts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8760" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Senvion" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>WEWW</t>
   </si>
   <si>
-    <t>WWWW</t>
-  </si>
-  <si>
     <t>EFCF</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>vfdsfv</t>
+  </si>
+  <si>
+    <t>NORDX-PRT-0001</t>
   </si>
 </sst>
 </file>
@@ -470,16 +470,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -625,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -648,7 +653,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed all and settings, still testing suzlon
</commit_message>
<xml_diff>
--- a/Test c#/Parts.xlsx
+++ b/Test c#/Parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Gamesa Part No.</t>
   </si>
@@ -78,9 +78,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>WEWW</t>
-  </si>
-  <si>
     <t>EFCF</t>
   </si>
   <si>
@@ -91,6 +88,15 @@
   </si>
   <si>
     <t>NORDX-PRT-0001</t>
+  </si>
+  <si>
+    <t>REPWR-PRT-0001</t>
+  </si>
+  <si>
+    <t>Nordex Part No</t>
+  </si>
+  <si>
+    <t>Mpulse Part No.</t>
   </si>
 </sst>
 </file>
@@ -444,6 +450,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -458,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -468,23 +477,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>